<commit_message>
correcoes no prj db-pipe
</commit_message>
<xml_diff>
--- a/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
+++ b/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Github/learn-python/PROJETOS/db-pipeline/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4D361C20488DEA4E38A093BC5F47C25BDEDD84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA7F596C-B4D5-4DC8-B635-77C8A8DD43EB}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="11_AD4D361C20488DEA4E38A093BC5F47C25BDEDD84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E749037-C6C5-4641-8BEE-982864FB5664}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>tabela</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>cols_originais</t>
-  </si>
-  <si>
-    <t>data_voo</t>
   </si>
   <si>
     <t>dep_time</t>
@@ -436,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,27 +456,27 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -488,16 +485,16 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -505,19 +502,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -531,13 +528,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -549,27 +546,27 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -583,25 +580,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -609,7 +606,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -630,70 +627,44 @@
         <v>0.05</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mudanca no print da arvore
</commit_message>
<xml_diff>
--- a/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
+++ b/PROJETOS/db-pipeline/assets/work_metadado_flights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Github/learn-python/PROJETOS/db-pipeline/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_AD4D361C20488DEA4E38A093BC5F47C25BDEDD84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90D3E81D-AB6E-40E0-BD5B-5BAFDAAA2649}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="11_AD4D361C20488DEA4E38A093BC5F47C25BDEDD84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3443CEFE-5955-4300-B4F4-9815EC8EF2BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21697" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>tabela</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>nyflights</t>
+  </si>
+  <si>
+    <t>origem</t>
+  </si>
+  <si>
+    <t>destino</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>dest</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -436,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -518,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -544,22 +559,22 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -573,22 +588,22 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -602,22 +617,22 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -631,25 +646,25 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -660,42 +675,100 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.05</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.05</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0.1</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>